<commit_message>
Fixed some ingredient names.
</commit_message>
<xml_diff>
--- a/Data/recipes/Data_UK_100.xlsx
+++ b/Data/recipes/Data_UK_100.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aslau\Desktop\UiBV21\Master\Data\oppskrifter\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aslau\Desktop\UiBV21\Master\R\sustainableRecipes\Data\recipes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFBB6EE2-DC52-4EB4-AF8B-B112BAD4F4E0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8704DA73-29F1-4FF7-B2C9-C535786A17E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12555" yWindow="1275" windowWidth="23760" windowHeight="12585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="339" uniqueCount="232">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="444" uniqueCount="233">
   <si>
     <t>kcal</t>
   </si>
@@ -371,17 +371,6 @@
 2 red onions
 2 tsp dried oregano
 1 stk orange zest</t>
-  </si>
-  <si>
-    <t>1 litre chicken stock
-0.4g saffron threads
-65 g butter
-15 ml tablespoon regular olive oil
-50 g shallots
-250 g risotto rice
-125 ml dry marsala
-30 g parmesan
-salt and pepper, to taste</t>
   </si>
   <si>
     <t>500 g potatoes
@@ -1720,9 +1709,6 @@
 6 tablespoons aged cider vinegar</t>
   </si>
   <si>
-    <t>Recipe says baby onions</t>
-  </si>
-  <si>
     <t>1 handful basil
 500 g ground meat beef
 1 tbsp mustard
@@ -1898,6 +1884,23 @@
 6 ounces puff pastry
 1 egg
 1 tablespoon parmesan</t>
+  </si>
+  <si>
+    <t>Country</t>
+  </si>
+  <si>
+    <t>UK</t>
+  </si>
+  <si>
+    <t>1 litre chicken stock
+0.4g saffron threads
+65 g butter
+15 ml regular olive oil
+50 g shallots
+250 g risotto rice
+125 ml dry marsala
+30 g parmesan
+salt and pepper, to taste</t>
   </si>
 </sst>
 </file>
@@ -2304,8 +2307,8 @@
   <dimension ref="A1:R106"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
+      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C46" sqref="C46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2314,7 +2317,7 @@
     <col min="2" max="2" width="32.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>109</v>
       </c>
@@ -2355,15 +2358,18 @@
         <v>9</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" ht="180" x14ac:dyDescent="0.25">
+        <v>158</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" ht="180" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>10</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="C2">
         <v>4</v>
@@ -2398,13 +2404,16 @@
       <c r="M2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="3" spans="1:15" ht="195" x14ac:dyDescent="0.25">
+      <c r="P2" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" ht="195" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>14</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C3">
         <v>4</v>
@@ -2439,13 +2448,16 @@
       <c r="M3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="4" spans="1:15" ht="210" x14ac:dyDescent="0.25">
+      <c r="P3" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" ht="210" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>16</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C4">
         <v>4</v>
@@ -2480,13 +2492,16 @@
       <c r="M4" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="5" spans="1:15" ht="240" x14ac:dyDescent="0.25">
+      <c r="P4" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" ht="240" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>38</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C5">
         <v>4</v>
@@ -2521,13 +2536,16 @@
       <c r="M5" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="6" spans="1:15" ht="135" x14ac:dyDescent="0.25">
+      <c r="P5" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" ht="135" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>41</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C6">
         <v>4</v>
@@ -2562,13 +2580,16 @@
       <c r="M6" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="7" spans="1:15" ht="135" x14ac:dyDescent="0.25">
+      <c r="P6" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" ht="135" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>44</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C7">
         <v>6</v>
@@ -2603,13 +2624,16 @@
       <c r="M7" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="8" spans="1:15" ht="285" x14ac:dyDescent="0.25">
+      <c r="P7" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" ht="285" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>51</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C8">
         <v>4</v>
@@ -2644,8 +2668,11 @@
       <c r="M8" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P8" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>16</v>
       </c>
@@ -2679,13 +2706,16 @@
       <c r="M9" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="10" spans="1:15" ht="225" x14ac:dyDescent="0.25">
+      <c r="P9" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" ht="225" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>53</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C10">
         <v>3</v>
@@ -2720,13 +2750,16 @@
       <c r="M10" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="11" spans="1:15" ht="225" x14ac:dyDescent="0.25">
+      <c r="P10" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" ht="225" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>59</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C11">
         <v>2</v>
@@ -2761,13 +2794,16 @@
       <c r="M11" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="12" spans="1:15" ht="255" x14ac:dyDescent="0.25">
+      <c r="P11" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" ht="255" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>63</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C12">
         <v>3</v>
@@ -2802,13 +2838,16 @@
       <c r="M12" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="13" spans="1:15" ht="210" x14ac:dyDescent="0.25">
+      <c r="P12" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" ht="210" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>71</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C13">
         <v>4</v>
@@ -2843,13 +2882,16 @@
       <c r="M13" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="14" spans="1:15" ht="195" x14ac:dyDescent="0.25">
+      <c r="P13" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" ht="195" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>149</v>
+      </c>
+      <c r="B14" s="2" t="s">
         <v>150</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>151</v>
       </c>
       <c r="C14">
         <v>2</v>
@@ -2884,13 +2926,16 @@
       <c r="M14" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="15" spans="1:15" ht="135" x14ac:dyDescent="0.25">
+      <c r="P14" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" ht="135" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>76</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C15">
         <v>5</v>
@@ -2925,13 +2970,16 @@
       <c r="M15" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="16" spans="1:15" ht="330" x14ac:dyDescent="0.25">
+      <c r="P15" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" ht="330" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>80</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C16">
         <v>4</v>
@@ -2965,6 +3013,9 @@
       </c>
       <c r="M16" t="s">
         <v>11</v>
+      </c>
+      <c r="P16" t="s">
+        <v>231</v>
       </c>
     </row>
     <row r="17" spans="1:16" ht="105" x14ac:dyDescent="0.25">
@@ -2972,7 +3023,7 @@
         <v>90</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C17">
         <v>4</v>
@@ -3006,6 +3057,9 @@
       </c>
       <c r="M17" t="s">
         <v>11</v>
+      </c>
+      <c r="P17" t="s">
+        <v>231</v>
       </c>
     </row>
     <row r="18" spans="1:16" ht="225" x14ac:dyDescent="0.25">
@@ -3013,7 +3067,7 @@
         <v>98</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C18">
         <v>4</v>
@@ -3047,6 +3101,9 @@
       </c>
       <c r="M18" t="s">
         <v>11</v>
+      </c>
+      <c r="P18" t="s">
+        <v>231</v>
       </c>
     </row>
     <row r="19" spans="1:16" ht="135" x14ac:dyDescent="0.25">
@@ -3054,7 +3111,7 @@
         <v>100</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C19">
         <v>4</v>
@@ -3090,7 +3147,7 @@
         <v>11</v>
       </c>
       <c r="P19" t="s">
-        <v>221</v>
+        <v>231</v>
       </c>
     </row>
     <row r="20" spans="1:16" ht="180" x14ac:dyDescent="0.25">
@@ -3098,7 +3155,7 @@
         <v>102</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C20">
         <v>2</v>
@@ -3132,6 +3189,9 @@
       </c>
       <c r="M20" t="s">
         <v>11</v>
+      </c>
+      <c r="P20" t="s">
+        <v>231</v>
       </c>
     </row>
     <row r="21" spans="1:16" ht="375" x14ac:dyDescent="0.25">
@@ -3139,7 +3199,7 @@
         <v>105</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C21">
         <v>4</v>
@@ -3173,6 +3233,9 @@
       </c>
       <c r="M21" t="s">
         <v>11</v>
+      </c>
+      <c r="P21" t="s">
+        <v>231</v>
       </c>
     </row>
     <row r="22" spans="1:16" ht="195" x14ac:dyDescent="0.25">
@@ -3180,7 +3243,7 @@
         <v>107</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C22">
         <v>3</v>
@@ -3214,6 +3277,9 @@
       </c>
       <c r="M22" t="s">
         <v>11</v>
+      </c>
+      <c r="P22" t="s">
+        <v>231</v>
       </c>
     </row>
     <row r="23" spans="1:16" ht="195" x14ac:dyDescent="0.25">
@@ -3221,7 +3287,7 @@
         <v>17</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C23">
         <v>2</v>
@@ -3255,6 +3321,9 @@
       </c>
       <c r="M23" t="s">
         <v>18</v>
+      </c>
+      <c r="P23" t="s">
+        <v>231</v>
       </c>
     </row>
     <row r="24" spans="1:16" ht="285" x14ac:dyDescent="0.25">
@@ -3262,7 +3331,7 @@
         <v>26</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C24">
         <v>4</v>
@@ -3296,6 +3365,9 @@
       </c>
       <c r="M24" t="s">
         <v>18</v>
+      </c>
+      <c r="P24" t="s">
+        <v>231</v>
       </c>
     </row>
     <row r="25" spans="1:16" ht="195" x14ac:dyDescent="0.25">
@@ -3303,7 +3375,7 @@
         <v>27</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C25">
         <v>2</v>
@@ -3337,6 +3409,9 @@
       </c>
       <c r="M25" t="s">
         <v>18</v>
+      </c>
+      <c r="P25" t="s">
+        <v>231</v>
       </c>
     </row>
     <row r="26" spans="1:16" ht="90" x14ac:dyDescent="0.25">
@@ -3344,7 +3419,7 @@
         <v>31</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C26">
         <v>4</v>
@@ -3378,6 +3453,9 @@
       </c>
       <c r="M26" t="s">
         <v>18</v>
+      </c>
+      <c r="P26" t="s">
+        <v>231</v>
       </c>
     </row>
     <row r="27" spans="1:16" ht="135" x14ac:dyDescent="0.25">
@@ -3385,7 +3463,7 @@
         <v>40</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C27">
         <v>4</v>
@@ -3419,6 +3497,9 @@
       </c>
       <c r="M27" t="s">
         <v>18</v>
+      </c>
+      <c r="P27" t="s">
+        <v>231</v>
       </c>
     </row>
     <row r="28" spans="1:16" ht="240" x14ac:dyDescent="0.25">
@@ -3426,7 +3507,7 @@
         <v>46</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C28">
         <v>2</v>
@@ -3460,6 +3541,9 @@
       </c>
       <c r="M28" t="s">
         <v>18</v>
+      </c>
+      <c r="P28" t="s">
+        <v>231</v>
       </c>
     </row>
     <row r="29" spans="1:16" ht="90" x14ac:dyDescent="0.25">
@@ -3467,7 +3551,7 @@
         <v>47</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C29">
         <v>2</v>
@@ -3501,6 +3585,9 @@
       </c>
       <c r="M29" t="s">
         <v>18</v>
+      </c>
+      <c r="P29" t="s">
+        <v>231</v>
       </c>
     </row>
     <row r="30" spans="1:16" ht="105" x14ac:dyDescent="0.25">
@@ -3508,7 +3595,7 @@
         <v>54</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C30">
         <v>4</v>
@@ -3542,6 +3629,9 @@
       </c>
       <c r="M30" t="s">
         <v>18</v>
+      </c>
+      <c r="P30" t="s">
+        <v>231</v>
       </c>
     </row>
     <row r="31" spans="1:16" ht="180" x14ac:dyDescent="0.25">
@@ -3549,7 +3639,7 @@
         <v>55</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C31">
         <v>2</v>
@@ -3583,6 +3673,9 @@
       </c>
       <c r="M31" t="s">
         <v>18</v>
+      </c>
+      <c r="P31" t="s">
+        <v>231</v>
       </c>
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.25">
@@ -3619,13 +3712,16 @@
       <c r="M32" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="33" spans="1:13" ht="165" x14ac:dyDescent="0.25">
+      <c r="P32" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="33" spans="1:16" ht="165" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>58</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C33">
         <v>4</v>
@@ -3660,13 +3756,16 @@
       <c r="M33" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="34" spans="1:13" ht="165" x14ac:dyDescent="0.25">
+      <c r="P33" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="34" spans="1:16" ht="165" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>62</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C34">
         <v>2</v>
@@ -3701,13 +3800,16 @@
       <c r="M34" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="35" spans="1:13" ht="165" x14ac:dyDescent="0.25">
+      <c r="P34" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="35" spans="1:16" ht="165" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>64</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C35">
         <v>4</v>
@@ -3742,13 +3844,16 @@
       <c r="M35" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="36" spans="1:13" ht="165" x14ac:dyDescent="0.25">
+      <c r="P35" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="36" spans="1:16" ht="165" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>67</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C36">
         <v>4</v>
@@ -3783,13 +3888,16 @@
       <c r="M36" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="37" spans="1:13" ht="165" x14ac:dyDescent="0.25">
+      <c r="P36" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="37" spans="1:16" ht="165" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>74</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="C37">
         <v>2</v>
@@ -3824,13 +3932,16 @@
       <c r="M37" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="38" spans="1:13" ht="150" x14ac:dyDescent="0.25">
+      <c r="P37" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="38" spans="1:16" ht="150" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>78</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C38">
         <v>2</v>
@@ -3865,13 +3976,16 @@
       <c r="M38" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="39" spans="1:13" ht="165" x14ac:dyDescent="0.25">
+      <c r="P38" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="39" spans="1:16" ht="165" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>81</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C39">
         <v>4</v>
@@ -3906,13 +4020,16 @@
       <c r="M39" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="40" spans="1:13" ht="270" x14ac:dyDescent="0.25">
+      <c r="P39" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="40" spans="1:16" ht="270" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>83</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C40">
         <v>2</v>
@@ -3947,13 +4064,16 @@
       <c r="M40" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="41" spans="1:13" ht="300" x14ac:dyDescent="0.25">
+      <c r="P40" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="41" spans="1:16" ht="300" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>92</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C41">
         <v>2</v>
@@ -3988,13 +4108,16 @@
       <c r="M41" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="42" spans="1:13" ht="255" x14ac:dyDescent="0.25">
+      <c r="P41" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="42" spans="1:16" ht="255" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>93</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C42">
         <v>4</v>
@@ -4029,13 +4152,16 @@
       <c r="M42" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="43" spans="1:13" ht="210" x14ac:dyDescent="0.25">
+      <c r="P42" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="43" spans="1:16" ht="210" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>95</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C43">
         <v>4</v>
@@ -4070,13 +4196,16 @@
       <c r="M43" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="44" spans="1:13" ht="135" x14ac:dyDescent="0.25">
+      <c r="P43" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="44" spans="1:16" ht="135" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>106</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C44">
         <v>2</v>
@@ -4111,8 +4240,11 @@
       <c r="M44" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="45" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+      <c r="P44" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="45" spans="1:16" ht="60" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>12</v>
       </c>
@@ -4152,13 +4284,16 @@
       <c r="M45" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="46" spans="1:13" ht="135" x14ac:dyDescent="0.25">
+      <c r="P45" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="46" spans="1:16" ht="135" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>15</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>114</v>
+        <v>232</v>
       </c>
       <c r="C46">
         <v>2</v>
@@ -4193,13 +4328,16 @@
       <c r="M46" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="47" spans="1:13" ht="120" x14ac:dyDescent="0.25">
+      <c r="P46" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="47" spans="1:16" ht="120" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>19</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C47">
         <v>6</v>
@@ -4234,8 +4372,11 @@
       <c r="M47" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="48" spans="1:13" ht="120" x14ac:dyDescent="0.25">
+      <c r="P47" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="48" spans="1:16" ht="120" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>20</v>
       </c>
@@ -4274,6 +4415,9 @@
       </c>
       <c r="M48" t="s">
         <v>13</v>
+      </c>
+      <c r="P48" t="s">
+        <v>231</v>
       </c>
     </row>
     <row r="49" spans="1:18" ht="105" x14ac:dyDescent="0.25">
@@ -4281,7 +4425,7 @@
         <v>24</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C49">
         <v>2</v>
@@ -4315,6 +4459,9 @@
       </c>
       <c r="M49" t="s">
         <v>13</v>
+      </c>
+      <c r="P49" t="s">
+        <v>231</v>
       </c>
     </row>
     <row r="50" spans="1:18" ht="105" x14ac:dyDescent="0.25">
@@ -4322,7 +4469,7 @@
         <v>28</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C50">
         <v>2</v>
@@ -4356,6 +4503,9 @@
       </c>
       <c r="M50" t="s">
         <v>13</v>
+      </c>
+      <c r="P50" t="s">
+        <v>231</v>
       </c>
     </row>
     <row r="51" spans="1:18" ht="150" x14ac:dyDescent="0.25">
@@ -4363,7 +4513,7 @@
         <v>35</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C51">
         <v>6</v>
@@ -4397,6 +4547,9 @@
       </c>
       <c r="M51" t="s">
         <v>13</v>
+      </c>
+      <c r="P51" t="s">
+        <v>231</v>
       </c>
     </row>
     <row r="52" spans="1:18" ht="150" x14ac:dyDescent="0.25">
@@ -4404,7 +4557,7 @@
         <v>37</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C52">
         <v>2</v>
@@ -4438,6 +4591,9 @@
       </c>
       <c r="M52" t="s">
         <v>13</v>
+      </c>
+      <c r="P52" t="s">
+        <v>231</v>
       </c>
     </row>
     <row r="53" spans="1:18" ht="255" x14ac:dyDescent="0.25">
@@ -4445,7 +4601,7 @@
         <v>42</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C53">
         <v>6</v>
@@ -4479,6 +4635,9 @@
       </c>
       <c r="M53" t="s">
         <v>13</v>
+      </c>
+      <c r="P53" t="s">
+        <v>231</v>
       </c>
     </row>
     <row r="54" spans="1:18" ht="135" x14ac:dyDescent="0.25">
@@ -4486,7 +4645,7 @@
         <v>43</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C54">
         <v>2</v>
@@ -4520,6 +4679,9 @@
       </c>
       <c r="M54" t="s">
         <v>13</v>
+      </c>
+      <c r="P54" t="s">
+        <v>231</v>
       </c>
     </row>
     <row r="55" spans="1:18" ht="165" x14ac:dyDescent="0.25">
@@ -4527,7 +4689,7 @@
         <v>45</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C55">
         <v>4</v>
@@ -4561,6 +4723,9 @@
       </c>
       <c r="M55" t="s">
         <v>13</v>
+      </c>
+      <c r="P55" t="s">
+        <v>231</v>
       </c>
     </row>
     <row r="56" spans="1:18" x14ac:dyDescent="0.25">
@@ -4597,13 +4762,16 @@
       <c r="M56" t="s">
         <v>13</v>
       </c>
+      <c r="P56" t="s">
+        <v>231</v>
+      </c>
     </row>
     <row r="57" spans="1:18" ht="150" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>48</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C57">
         <v>6</v>
@@ -4637,6 +4805,9 @@
       </c>
       <c r="M57" t="s">
         <v>13</v>
+      </c>
+      <c r="P57" t="s">
+        <v>231</v>
       </c>
     </row>
     <row r="58" spans="1:18" ht="240" x14ac:dyDescent="0.25">
@@ -4644,7 +4815,7 @@
         <v>49</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C58">
         <v>4</v>
@@ -4678,6 +4849,9 @@
       </c>
       <c r="M58" t="s">
         <v>13</v>
+      </c>
+      <c r="P58" t="s">
+        <v>231</v>
       </c>
       <c r="R58" s="2"/>
     </row>
@@ -4686,7 +4860,7 @@
         <v>50</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C59">
         <v>8</v>
@@ -4720,6 +4894,9 @@
       </c>
       <c r="M59" t="s">
         <v>13</v>
+      </c>
+      <c r="P59" t="s">
+        <v>231</v>
       </c>
     </row>
     <row r="60" spans="1:18" ht="255" x14ac:dyDescent="0.25">
@@ -4727,7 +4904,7 @@
         <v>57</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C60">
         <v>4</v>
@@ -4761,6 +4938,9 @@
       </c>
       <c r="M60" t="s">
         <v>13</v>
+      </c>
+      <c r="P60" t="s">
+        <v>231</v>
       </c>
     </row>
     <row r="61" spans="1:18" ht="180" x14ac:dyDescent="0.25">
@@ -4768,7 +4948,7 @@
         <v>68</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C61">
         <v>4</v>
@@ -4802,6 +4982,9 @@
       </c>
       <c r="M61" t="s">
         <v>13</v>
+      </c>
+      <c r="P61" t="s">
+        <v>231</v>
       </c>
       <c r="R61" s="2"/>
     </row>
@@ -4810,7 +4993,7 @@
         <v>69</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C62">
         <v>4</v>
@@ -4844,6 +5027,9 @@
       </c>
       <c r="M62" t="s">
         <v>13</v>
+      </c>
+      <c r="P62" t="s">
+        <v>231</v>
       </c>
     </row>
     <row r="63" spans="1:18" ht="195" x14ac:dyDescent="0.25">
@@ -4851,7 +5037,7 @@
         <v>70</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C63">
         <v>6</v>
@@ -4885,6 +5071,9 @@
       </c>
       <c r="M63" t="s">
         <v>13</v>
+      </c>
+      <c r="P63" t="s">
+        <v>231</v>
       </c>
     </row>
     <row r="64" spans="1:18" ht="225" x14ac:dyDescent="0.25">
@@ -4892,7 +5081,7 @@
         <v>72</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C64">
         <v>8</v>
@@ -4927,13 +5116,16 @@
       <c r="M64" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="65" spans="1:15" ht="195" x14ac:dyDescent="0.25">
+      <c r="P64" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="65" spans="1:16" ht="195" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>73</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C65">
         <v>6</v>
@@ -4968,13 +5160,16 @@
       <c r="M65" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="66" spans="1:15" ht="135" x14ac:dyDescent="0.25">
+      <c r="P65" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="66" spans="1:16" ht="135" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>77</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C66">
         <v>6</v>
@@ -5009,13 +5204,16 @@
       <c r="M66" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="67" spans="1:15" ht="105" x14ac:dyDescent="0.25">
+      <c r="P66" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="67" spans="1:16" ht="105" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>85</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C67">
         <v>3</v>
@@ -5050,13 +5248,16 @@
       <c r="M67" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="68" spans="1:15" ht="285" x14ac:dyDescent="0.25">
+      <c r="P67" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="68" spans="1:16" ht="285" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>89</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C68">
         <v>4</v>
@@ -5091,13 +5292,16 @@
       <c r="M68" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="69" spans="1:15" ht="240" x14ac:dyDescent="0.25">
+      <c r="P68" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="69" spans="1:16" ht="240" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>108</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C69">
         <v>8</v>
@@ -5132,13 +5336,16 @@
       <c r="M69" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="70" spans="1:15" ht="255" x14ac:dyDescent="0.25">
+      <c r="P69" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="70" spans="1:16" ht="255" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>29</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C70">
         <v>4</v>
@@ -5173,13 +5380,16 @@
       <c r="M70" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="71" spans="1:15" ht="315" x14ac:dyDescent="0.25">
+      <c r="P70" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="71" spans="1:16" ht="315" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>32</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C71">
         <v>4</v>
@@ -5214,13 +5424,16 @@
       <c r="M71" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="72" spans="1:15" ht="330" x14ac:dyDescent="0.25">
+      <c r="P71" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="72" spans="1:16" ht="330" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>65</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C72">
         <v>4</v>
@@ -5255,8 +5468,11 @@
       <c r="M72" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="73" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P72" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="73" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>29</v>
       </c>
@@ -5290,13 +5506,16 @@
       <c r="M73" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="74" spans="1:15" ht="180" x14ac:dyDescent="0.25">
+      <c r="P73" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="74" spans="1:16" ht="180" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>86</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C74">
         <v>4</v>
@@ -5331,13 +5550,16 @@
       <c r="M74" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="75" spans="1:15" ht="165" x14ac:dyDescent="0.25">
+      <c r="P74" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="75" spans="1:16" ht="165" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>97</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C75">
         <v>8</v>
@@ -5372,13 +5594,16 @@
       <c r="M75" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="76" spans="1:15" ht="210" x14ac:dyDescent="0.25">
+      <c r="P75" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="76" spans="1:16" ht="210" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>99</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="C76">
         <v>4</v>
@@ -5414,15 +5639,18 @@
         <v>30</v>
       </c>
       <c r="O76" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="77" spans="1:15" ht="375" x14ac:dyDescent="0.25">
+        <v>224</v>
+      </c>
+      <c r="P76" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="77" spans="1:16" ht="375" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>21</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="C77">
         <v>6</v>
@@ -5458,15 +5686,18 @@
         <v>22</v>
       </c>
       <c r="O77" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="78" spans="1:15" ht="330" x14ac:dyDescent="0.25">
+        <v>159</v>
+      </c>
+      <c r="P77" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="78" spans="1:16" ht="330" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>23</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C78">
         <v>4</v>
@@ -5501,13 +5732,16 @@
       <c r="M78" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="79" spans="1:15" ht="405" x14ac:dyDescent="0.25">
+      <c r="P78" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="79" spans="1:16" ht="405" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>25</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C79">
         <v>4</v>
@@ -5543,15 +5777,18 @@
         <v>22</v>
       </c>
       <c r="O79" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="80" spans="1:15" ht="270" x14ac:dyDescent="0.25">
+        <v>161</v>
+      </c>
+      <c r="P79" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="80" spans="1:16" ht="270" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>33</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C80">
         <v>6</v>
@@ -5586,13 +5823,16 @@
       <c r="M80" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="81" spans="1:15" ht="240" x14ac:dyDescent="0.25">
+      <c r="P80" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="81" spans="1:16" ht="240" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>34</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C81">
         <v>4</v>
@@ -5627,13 +5867,16 @@
       <c r="M81" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="82" spans="1:15" ht="270" x14ac:dyDescent="0.25">
+      <c r="P81" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="82" spans="1:16" ht="270" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>36</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="C82">
         <v>4</v>
@@ -5669,15 +5912,18 @@
         <v>22</v>
       </c>
       <c r="O82" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="83" spans="1:15" ht="345" x14ac:dyDescent="0.25">
+        <v>169</v>
+      </c>
+      <c r="P82" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="83" spans="1:16" ht="345" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>39</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C83">
         <v>4</v>
@@ -5713,15 +5959,18 @@
         <v>22</v>
       </c>
       <c r="O83" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="84" spans="1:15" ht="330" x14ac:dyDescent="0.25">
+        <v>165</v>
+      </c>
+      <c r="P83" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="84" spans="1:16" ht="330" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>52</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C84">
         <v>4</v>
@@ -5756,13 +6005,16 @@
       <c r="M84" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="85" spans="1:15" ht="285" x14ac:dyDescent="0.25">
+      <c r="P84" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="85" spans="1:16" ht="285" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>56</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C85">
         <v>4</v>
@@ -5797,13 +6049,16 @@
       <c r="M85" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="86" spans="1:15" ht="240" x14ac:dyDescent="0.25">
+      <c r="P85" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="86" spans="1:16" ht="240" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>60</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C86">
         <v>4</v>
@@ -5839,15 +6094,18 @@
         <v>22</v>
       </c>
       <c r="O86" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="87" spans="1:15" ht="285" x14ac:dyDescent="0.25">
+        <v>161</v>
+      </c>
+      <c r="P86" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="87" spans="1:16" ht="285" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>61</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="C87">
         <v>4</v>
@@ -5883,15 +6141,18 @@
         <v>22</v>
       </c>
       <c r="O87" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="88" spans="1:15" ht="330" x14ac:dyDescent="0.25">
+        <v>161</v>
+      </c>
+      <c r="P87" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="88" spans="1:16" ht="330" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>66</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C88">
         <v>4</v>
@@ -5926,13 +6187,16 @@
       <c r="M88" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="89" spans="1:15" ht="210" x14ac:dyDescent="0.25">
+      <c r="P88" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="89" spans="1:16" ht="210" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>75</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C89">
         <v>4</v>
@@ -5967,13 +6231,16 @@
       <c r="M89" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="90" spans="1:15" ht="165" x14ac:dyDescent="0.25">
+      <c r="P89" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="90" spans="1:16" ht="165" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>79</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C90">
         <v>4</v>
@@ -6008,13 +6275,16 @@
       <c r="M90" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="91" spans="1:15" ht="240" x14ac:dyDescent="0.25">
+      <c r="P90" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="91" spans="1:16" ht="240" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>82</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C91">
         <v>4</v>
@@ -6049,13 +6319,16 @@
       <c r="M91" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="92" spans="1:15" ht="210" x14ac:dyDescent="0.25">
+      <c r="P91" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="92" spans="1:16" ht="210" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>84</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C92">
         <v>6</v>
@@ -6090,13 +6363,16 @@
       <c r="M92" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="93" spans="1:15" ht="240" x14ac:dyDescent="0.25">
+      <c r="P92" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="93" spans="1:16" ht="240" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>87</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C93">
         <v>6</v>
@@ -6131,13 +6407,16 @@
       <c r="M93" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="94" spans="1:15" ht="255" x14ac:dyDescent="0.25">
+      <c r="P93" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="94" spans="1:16" ht="255" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>88</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C94">
         <v>6</v>
@@ -6172,13 +6451,16 @@
       <c r="M94" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="95" spans="1:15" ht="270" x14ac:dyDescent="0.25">
+      <c r="P94" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="95" spans="1:16" ht="270" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>91</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C95">
         <v>4</v>
@@ -6214,15 +6496,18 @@
         <v>22</v>
       </c>
       <c r="O95" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="96" spans="1:15" ht="315" x14ac:dyDescent="0.25">
+        <v>178</v>
+      </c>
+      <c r="P95" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="96" spans="1:16" ht="315" x14ac:dyDescent="0.25">
       <c r="A96" s="5" t="s">
         <v>94</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="C96">
         <v>4</v>
@@ -6257,13 +6542,16 @@
       <c r="M96" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="97" spans="1:15" ht="270" x14ac:dyDescent="0.25">
+      <c r="P96" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="97" spans="1:16" ht="270" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>96</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C97">
         <v>4</v>
@@ -6298,13 +6586,16 @@
       <c r="M97" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="98" spans="1:15" ht="330" x14ac:dyDescent="0.25">
+      <c r="P97" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="98" spans="1:16" ht="330" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>101</v>
       </c>
       <c r="B98" s="3" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="C98">
         <v>4</v>
@@ -6340,15 +6631,18 @@
         <v>22</v>
       </c>
       <c r="O98" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="99" spans="1:15" ht="270" x14ac:dyDescent="0.25">
+        <v>180</v>
+      </c>
+      <c r="P98" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="99" spans="1:16" ht="270" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>103</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="C99" s="6">
         <v>6</v>
@@ -6383,13 +6677,16 @@
       <c r="M99" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="100" spans="1:15" ht="315" x14ac:dyDescent="0.25">
+      <c r="P99" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="100" spans="1:16" ht="315" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>104</v>
       </c>
       <c r="B100" s="3" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C100">
         <v>4</v>
@@ -6425,10 +6722,13 @@
         <v>22</v>
       </c>
       <c r="O100" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="101" spans="1:15" x14ac:dyDescent="0.25">
+        <v>182</v>
+      </c>
+      <c r="P100" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="101" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>79</v>
       </c>
@@ -6462,13 +6762,16 @@
       <c r="M101" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="102" spans="1:15" ht="135" x14ac:dyDescent="0.25">
+      <c r="P101" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="102" spans="1:16" ht="135" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
+        <v>205</v>
+      </c>
+      <c r="B102" s="2" t="s">
         <v>206</v>
-      </c>
-      <c r="B102" s="2" t="s">
-        <v>207</v>
       </c>
       <c r="C102">
         <v>4</v>
@@ -6476,13 +6779,16 @@
       <c r="M102" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="103" spans="1:15" ht="390" x14ac:dyDescent="0.25">
+      <c r="P102" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="103" spans="1:16" ht="390" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B103" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C103">
         <v>4</v>
@@ -6491,15 +6797,18 @@
         <v>30</v>
       </c>
       <c r="O103" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="P103" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="104" spans="1:16" ht="330" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
         <v>209</v>
       </c>
-    </row>
-    <row r="104" spans="1:15" ht="330" x14ac:dyDescent="0.25">
-      <c r="A104" t="s">
-        <v>210</v>
-      </c>
       <c r="B104" s="2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C104">
         <v>4</v>
@@ -6508,15 +6817,18 @@
         <v>22</v>
       </c>
       <c r="O104" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="105" spans="1:15" ht="240" x14ac:dyDescent="0.25">
+        <v>210</v>
+      </c>
+      <c r="P104" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="105" spans="1:16" ht="240" x14ac:dyDescent="0.25">
       <c r="A105" s="4" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B105" s="2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C105">
         <v>2</v>
@@ -6525,15 +6837,18 @@
         <v>18</v>
       </c>
       <c r="O105" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="106" spans="1:15" ht="90" x14ac:dyDescent="0.25">
+        <v>213</v>
+      </c>
+      <c r="P105" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="106" spans="1:16" ht="90" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
+        <v>216</v>
+      </c>
+      <c r="B106" s="2" t="s">
         <v>217</v>
-      </c>
-      <c r="B106" s="2" t="s">
-        <v>218</v>
       </c>
       <c r="C106">
         <v>4</v>
@@ -6542,7 +6857,10 @@
         <v>13</v>
       </c>
       <c r="O106" t="s">
-        <v>219</v>
+        <v>218</v>
+      </c>
+      <c r="P106" t="s">
+        <v>231</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed missing ingredient name.
</commit_message>
<xml_diff>
--- a/Data/recipes/Data_UK_100.xlsx
+++ b/Data/recipes/Data_UK_100.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24430"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aslau\Desktop\UiBV21\Master\R\sustainableRecipes\Data\recipes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8704DA73-29F1-4FF7-B2C9-C535786A17E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67909FEF-39C0-41E4-881E-8ABC1A2384CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3045" yWindow="1440" windowWidth="23760" windowHeight="12585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -851,13 +851,6 @@
 1 pinch of cayenne pepper 
 1 teaspoon very finely chopped fresh thyme (optional)
 Sunflower or peanut oil for frying</t>
-  </si>
-  <si>
-    <t>1 pound potatoes
-3 handfuls of sorrel, cultivated or wild
-3 tablespoons unsalted butter
-1 tablespoon extra-virgin olive
-Fine sea salt and freshly ground black pepper</t>
   </si>
   <si>
     <t>⅓ cup hazelnuts
@@ -1901,6 +1894,13 @@
 125 ml dry marsala
 30 g parmesan
 salt and pepper, to taste</t>
+  </si>
+  <si>
+    <t>1 pound potatoes
+3 handfuls of sorrel, cultivated or wild
+3 tablespoons unsalted butter
+1 tablespoon extra-virgin olive oil
+Fine sea salt and freshly ground black pepper</t>
   </si>
 </sst>
 </file>
@@ -2307,8 +2307,8 @@
   <dimension ref="A1:R106"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C46" sqref="C46"/>
+      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2358,10 +2358,10 @@
         <v>9</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="2" spans="1:16" ht="180" x14ac:dyDescent="0.25">
@@ -2369,7 +2369,7 @@
         <v>10</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C2">
         <v>4</v>
@@ -2405,7 +2405,7 @@
         <v>11</v>
       </c>
       <c r="P2" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="3" spans="1:16" ht="195" x14ac:dyDescent="0.25">
@@ -2449,7 +2449,7 @@
         <v>11</v>
       </c>
       <c r="P3" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="4" spans="1:16" ht="210" x14ac:dyDescent="0.25">
@@ -2493,7 +2493,7 @@
         <v>11</v>
       </c>
       <c r="P4" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="5" spans="1:16" ht="240" x14ac:dyDescent="0.25">
@@ -2537,7 +2537,7 @@
         <v>11</v>
       </c>
       <c r="P5" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="6" spans="1:16" ht="135" x14ac:dyDescent="0.25">
@@ -2581,7 +2581,7 @@
         <v>11</v>
       </c>
       <c r="P6" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="7" spans="1:16" ht="135" x14ac:dyDescent="0.25">
@@ -2625,7 +2625,7 @@
         <v>11</v>
       </c>
       <c r="P7" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="8" spans="1:16" ht="285" x14ac:dyDescent="0.25">
@@ -2669,7 +2669,7 @@
         <v>11</v>
       </c>
       <c r="P8" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
@@ -2707,7 +2707,7 @@
         <v>11</v>
       </c>
       <c r="P9" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="10" spans="1:16" ht="225" x14ac:dyDescent="0.25">
@@ -2751,7 +2751,7 @@
         <v>11</v>
       </c>
       <c r="P10" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="11" spans="1:16" ht="225" x14ac:dyDescent="0.25">
@@ -2795,7 +2795,7 @@
         <v>11</v>
       </c>
       <c r="P11" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="12" spans="1:16" ht="255" x14ac:dyDescent="0.25">
@@ -2839,7 +2839,7 @@
         <v>11</v>
       </c>
       <c r="P12" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="13" spans="1:16" ht="210" x14ac:dyDescent="0.25">
@@ -2883,7 +2883,7 @@
         <v>11</v>
       </c>
       <c r="P13" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="14" spans="1:16" ht="195" x14ac:dyDescent="0.25">
@@ -2927,7 +2927,7 @@
         <v>11</v>
       </c>
       <c r="P14" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="15" spans="1:16" ht="135" x14ac:dyDescent="0.25">
@@ -2971,7 +2971,7 @@
         <v>11</v>
       </c>
       <c r="P15" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="16" spans="1:16" ht="330" x14ac:dyDescent="0.25">
@@ -3015,7 +3015,7 @@
         <v>11</v>
       </c>
       <c r="P16" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="17" spans="1:16" ht="105" x14ac:dyDescent="0.25">
@@ -3023,7 +3023,7 @@
         <v>90</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>153</v>
+        <v>232</v>
       </c>
       <c r="C17">
         <v>4</v>
@@ -3059,7 +3059,7 @@
         <v>11</v>
       </c>
       <c r="P17" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="18" spans="1:16" ht="225" x14ac:dyDescent="0.25">
@@ -3067,7 +3067,7 @@
         <v>98</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C18">
         <v>4</v>
@@ -3103,7 +3103,7 @@
         <v>11</v>
       </c>
       <c r="P18" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="19" spans="1:16" ht="135" x14ac:dyDescent="0.25">
@@ -3111,7 +3111,7 @@
         <v>100</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C19">
         <v>4</v>
@@ -3147,7 +3147,7 @@
         <v>11</v>
       </c>
       <c r="P19" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="20" spans="1:16" ht="180" x14ac:dyDescent="0.25">
@@ -3155,7 +3155,7 @@
         <v>102</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C20">
         <v>2</v>
@@ -3191,7 +3191,7 @@
         <v>11</v>
       </c>
       <c r="P20" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="21" spans="1:16" ht="375" x14ac:dyDescent="0.25">
@@ -3199,7 +3199,7 @@
         <v>105</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C21">
         <v>4</v>
@@ -3235,7 +3235,7 @@
         <v>11</v>
       </c>
       <c r="P21" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="22" spans="1:16" ht="195" x14ac:dyDescent="0.25">
@@ -3243,7 +3243,7 @@
         <v>107</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C22">
         <v>3</v>
@@ -3279,7 +3279,7 @@
         <v>11</v>
       </c>
       <c r="P22" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="23" spans="1:16" ht="195" x14ac:dyDescent="0.25">
@@ -3287,7 +3287,7 @@
         <v>17</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C23">
         <v>2</v>
@@ -3323,7 +3323,7 @@
         <v>18</v>
       </c>
       <c r="P23" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="24" spans="1:16" ht="285" x14ac:dyDescent="0.25">
@@ -3331,7 +3331,7 @@
         <v>26</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C24">
         <v>4</v>
@@ -3367,7 +3367,7 @@
         <v>18</v>
       </c>
       <c r="P24" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="25" spans="1:16" ht="195" x14ac:dyDescent="0.25">
@@ -3375,7 +3375,7 @@
         <v>27</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C25">
         <v>2</v>
@@ -3411,7 +3411,7 @@
         <v>18</v>
       </c>
       <c r="P25" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="26" spans="1:16" ht="90" x14ac:dyDescent="0.25">
@@ -3419,7 +3419,7 @@
         <v>31</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C26">
         <v>4</v>
@@ -3455,7 +3455,7 @@
         <v>18</v>
       </c>
       <c r="P26" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="27" spans="1:16" ht="135" x14ac:dyDescent="0.25">
@@ -3463,7 +3463,7 @@
         <v>40</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C27">
         <v>4</v>
@@ -3499,7 +3499,7 @@
         <v>18</v>
       </c>
       <c r="P27" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="28" spans="1:16" ht="240" x14ac:dyDescent="0.25">
@@ -3507,7 +3507,7 @@
         <v>46</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C28">
         <v>2</v>
@@ -3543,7 +3543,7 @@
         <v>18</v>
       </c>
       <c r="P28" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="29" spans="1:16" ht="90" x14ac:dyDescent="0.25">
@@ -3551,7 +3551,7 @@
         <v>47</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C29">
         <v>2</v>
@@ -3587,7 +3587,7 @@
         <v>18</v>
       </c>
       <c r="P29" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="30" spans="1:16" ht="105" x14ac:dyDescent="0.25">
@@ -3595,7 +3595,7 @@
         <v>54</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C30">
         <v>4</v>
@@ -3631,7 +3631,7 @@
         <v>18</v>
       </c>
       <c r="P30" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="31" spans="1:16" ht="180" x14ac:dyDescent="0.25">
@@ -3639,7 +3639,7 @@
         <v>55</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C31">
         <v>2</v>
@@ -3675,7 +3675,7 @@
         <v>18</v>
       </c>
       <c r="P31" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.25">
@@ -3713,7 +3713,7 @@
         <v>18</v>
       </c>
       <c r="P32" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="33" spans="1:16" ht="165" x14ac:dyDescent="0.25">
@@ -3721,7 +3721,7 @@
         <v>58</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C33">
         <v>4</v>
@@ -3757,7 +3757,7 @@
         <v>18</v>
       </c>
       <c r="P33" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="34" spans="1:16" ht="165" x14ac:dyDescent="0.25">
@@ -3765,7 +3765,7 @@
         <v>62</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C34">
         <v>2</v>
@@ -3801,7 +3801,7 @@
         <v>18</v>
       </c>
       <c r="P34" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="35" spans="1:16" ht="165" x14ac:dyDescent="0.25">
@@ -3809,7 +3809,7 @@
         <v>64</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C35">
         <v>4</v>
@@ -3845,7 +3845,7 @@
         <v>18</v>
       </c>
       <c r="P35" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="36" spans="1:16" ht="165" x14ac:dyDescent="0.25">
@@ -3853,7 +3853,7 @@
         <v>67</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C36">
         <v>4</v>
@@ -3889,7 +3889,7 @@
         <v>18</v>
       </c>
       <c r="P36" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="37" spans="1:16" ht="165" x14ac:dyDescent="0.25">
@@ -3897,7 +3897,7 @@
         <v>74</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C37">
         <v>2</v>
@@ -3933,7 +3933,7 @@
         <v>18</v>
       </c>
       <c r="P37" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="38" spans="1:16" ht="150" x14ac:dyDescent="0.25">
@@ -3941,7 +3941,7 @@
         <v>78</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C38">
         <v>2</v>
@@ -3977,7 +3977,7 @@
         <v>18</v>
       </c>
       <c r="P38" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="39" spans="1:16" ht="165" x14ac:dyDescent="0.25">
@@ -3985,7 +3985,7 @@
         <v>81</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C39">
         <v>4</v>
@@ -4021,7 +4021,7 @@
         <v>18</v>
       </c>
       <c r="P39" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="40" spans="1:16" ht="270" x14ac:dyDescent="0.25">
@@ -4029,7 +4029,7 @@
         <v>83</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C40">
         <v>2</v>
@@ -4065,7 +4065,7 @@
         <v>18</v>
       </c>
       <c r="P40" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="41" spans="1:16" ht="300" x14ac:dyDescent="0.25">
@@ -4073,7 +4073,7 @@
         <v>92</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C41">
         <v>2</v>
@@ -4109,7 +4109,7 @@
         <v>18</v>
       </c>
       <c r="P41" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="42" spans="1:16" ht="255" x14ac:dyDescent="0.25">
@@ -4117,7 +4117,7 @@
         <v>93</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C42">
         <v>4</v>
@@ -4153,7 +4153,7 @@
         <v>18</v>
       </c>
       <c r="P42" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="43" spans="1:16" ht="210" x14ac:dyDescent="0.25">
@@ -4161,7 +4161,7 @@
         <v>95</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C43">
         <v>4</v>
@@ -4197,7 +4197,7 @@
         <v>18</v>
       </c>
       <c r="P43" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="44" spans="1:16" ht="135" x14ac:dyDescent="0.25">
@@ -4205,7 +4205,7 @@
         <v>106</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C44">
         <v>2</v>
@@ -4241,7 +4241,7 @@
         <v>18</v>
       </c>
       <c r="P44" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="45" spans="1:16" ht="60" x14ac:dyDescent="0.25">
@@ -4285,7 +4285,7 @@
         <v>13</v>
       </c>
       <c r="P45" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="46" spans="1:16" ht="135" x14ac:dyDescent="0.25">
@@ -4293,7 +4293,7 @@
         <v>15</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C46">
         <v>2</v>
@@ -4329,7 +4329,7 @@
         <v>13</v>
       </c>
       <c r="P46" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="47" spans="1:16" ht="120" x14ac:dyDescent="0.25">
@@ -4373,7 +4373,7 @@
         <v>13</v>
       </c>
       <c r="P47" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="48" spans="1:16" ht="120" x14ac:dyDescent="0.25">
@@ -4417,7 +4417,7 @@
         <v>13</v>
       </c>
       <c r="P48" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="49" spans="1:18" ht="105" x14ac:dyDescent="0.25">
@@ -4461,7 +4461,7 @@
         <v>13</v>
       </c>
       <c r="P49" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="50" spans="1:18" ht="105" x14ac:dyDescent="0.25">
@@ -4505,7 +4505,7 @@
         <v>13</v>
       </c>
       <c r="P50" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="51" spans="1:18" ht="150" x14ac:dyDescent="0.25">
@@ -4549,7 +4549,7 @@
         <v>13</v>
       </c>
       <c r="P51" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="52" spans="1:18" ht="150" x14ac:dyDescent="0.25">
@@ -4593,7 +4593,7 @@
         <v>13</v>
       </c>
       <c r="P52" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="53" spans="1:18" ht="255" x14ac:dyDescent="0.25">
@@ -4637,7 +4637,7 @@
         <v>13</v>
       </c>
       <c r="P53" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="54" spans="1:18" ht="135" x14ac:dyDescent="0.25">
@@ -4681,7 +4681,7 @@
         <v>13</v>
       </c>
       <c r="P54" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="55" spans="1:18" ht="165" x14ac:dyDescent="0.25">
@@ -4725,7 +4725,7 @@
         <v>13</v>
       </c>
       <c r="P55" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="56" spans="1:18" x14ac:dyDescent="0.25">
@@ -4763,7 +4763,7 @@
         <v>13</v>
       </c>
       <c r="P56" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="57" spans="1:18" ht="150" x14ac:dyDescent="0.25">
@@ -4807,7 +4807,7 @@
         <v>13</v>
       </c>
       <c r="P57" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="58" spans="1:18" ht="240" x14ac:dyDescent="0.25">
@@ -4851,7 +4851,7 @@
         <v>13</v>
       </c>
       <c r="P58" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="R58" s="2"/>
     </row>
@@ -4896,7 +4896,7 @@
         <v>13</v>
       </c>
       <c r="P59" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="60" spans="1:18" ht="255" x14ac:dyDescent="0.25">
@@ -4904,7 +4904,7 @@
         <v>57</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C60">
         <v>4</v>
@@ -4940,7 +4940,7 @@
         <v>13</v>
       </c>
       <c r="P60" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="61" spans="1:18" ht="180" x14ac:dyDescent="0.25">
@@ -4984,7 +4984,7 @@
         <v>13</v>
       </c>
       <c r="P61" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="R61" s="2"/>
     </row>
@@ -5029,7 +5029,7 @@
         <v>13</v>
       </c>
       <c r="P62" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="63" spans="1:18" ht="195" x14ac:dyDescent="0.25">
@@ -5073,7 +5073,7 @@
         <v>13</v>
       </c>
       <c r="P63" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="64" spans="1:18" ht="225" x14ac:dyDescent="0.25">
@@ -5117,7 +5117,7 @@
         <v>13</v>
       </c>
       <c r="P64" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="65" spans="1:16" ht="195" x14ac:dyDescent="0.25">
@@ -5161,7 +5161,7 @@
         <v>13</v>
       </c>
       <c r="P65" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="66" spans="1:16" ht="135" x14ac:dyDescent="0.25">
@@ -5205,7 +5205,7 @@
         <v>13</v>
       </c>
       <c r="P66" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="67" spans="1:16" ht="105" x14ac:dyDescent="0.25">
@@ -5249,7 +5249,7 @@
         <v>13</v>
       </c>
       <c r="P67" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="68" spans="1:16" ht="285" x14ac:dyDescent="0.25">
@@ -5293,7 +5293,7 @@
         <v>13</v>
       </c>
       <c r="P68" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="69" spans="1:16" ht="240" x14ac:dyDescent="0.25">
@@ -5337,7 +5337,7 @@
         <v>13</v>
       </c>
       <c r="P69" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="70" spans="1:16" ht="255" x14ac:dyDescent="0.25">
@@ -5381,7 +5381,7 @@
         <v>30</v>
       </c>
       <c r="P70" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="71" spans="1:16" ht="315" x14ac:dyDescent="0.25">
@@ -5425,7 +5425,7 @@
         <v>30</v>
       </c>
       <c r="P71" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="72" spans="1:16" ht="330" x14ac:dyDescent="0.25">
@@ -5469,7 +5469,7 @@
         <v>30</v>
       </c>
       <c r="P72" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="73" spans="1:16" x14ac:dyDescent="0.25">
@@ -5507,7 +5507,7 @@
         <v>30</v>
       </c>
       <c r="P73" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="74" spans="1:16" ht="180" x14ac:dyDescent="0.25">
@@ -5551,7 +5551,7 @@
         <v>30</v>
       </c>
       <c r="P74" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="75" spans="1:16" ht="165" x14ac:dyDescent="0.25">
@@ -5595,7 +5595,7 @@
         <v>30</v>
       </c>
       <c r="P75" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="76" spans="1:16" ht="210" x14ac:dyDescent="0.25">
@@ -5603,7 +5603,7 @@
         <v>99</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C76">
         <v>4</v>
@@ -5639,10 +5639,10 @@
         <v>30</v>
       </c>
       <c r="O76" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="P76" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="77" spans="1:16" ht="375" x14ac:dyDescent="0.25">
@@ -5650,7 +5650,7 @@
         <v>21</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C77">
         <v>6</v>
@@ -5686,10 +5686,10 @@
         <v>22</v>
       </c>
       <c r="O77" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="P77" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="78" spans="1:16" ht="330" x14ac:dyDescent="0.25">
@@ -5697,7 +5697,7 @@
         <v>23</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C78">
         <v>4</v>
@@ -5733,7 +5733,7 @@
         <v>22</v>
       </c>
       <c r="P78" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="79" spans="1:16" ht="405" x14ac:dyDescent="0.25">
@@ -5741,7 +5741,7 @@
         <v>25</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C79">
         <v>4</v>
@@ -5777,10 +5777,10 @@
         <v>22</v>
       </c>
       <c r="O79" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="P79" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="80" spans="1:16" ht="270" x14ac:dyDescent="0.25">
@@ -5788,7 +5788,7 @@
         <v>33</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C80">
         <v>6</v>
@@ -5824,7 +5824,7 @@
         <v>22</v>
       </c>
       <c r="P80" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="81" spans="1:16" ht="240" x14ac:dyDescent="0.25">
@@ -5832,7 +5832,7 @@
         <v>34</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C81">
         <v>4</v>
@@ -5868,7 +5868,7 @@
         <v>22</v>
       </c>
       <c r="P81" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="82" spans="1:16" ht="270" x14ac:dyDescent="0.25">
@@ -5876,7 +5876,7 @@
         <v>36</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C82">
         <v>4</v>
@@ -5912,10 +5912,10 @@
         <v>22</v>
       </c>
       <c r="O82" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="P82" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="83" spans="1:16" ht="345" x14ac:dyDescent="0.25">
@@ -5923,7 +5923,7 @@
         <v>39</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C83">
         <v>4</v>
@@ -5959,10 +5959,10 @@
         <v>22</v>
       </c>
       <c r="O83" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="P83" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="84" spans="1:16" ht="330" x14ac:dyDescent="0.25">
@@ -5970,7 +5970,7 @@
         <v>52</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C84">
         <v>4</v>
@@ -6006,7 +6006,7 @@
         <v>22</v>
       </c>
       <c r="P84" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="85" spans="1:16" ht="285" x14ac:dyDescent="0.25">
@@ -6014,7 +6014,7 @@
         <v>56</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C85">
         <v>4</v>
@@ -6050,7 +6050,7 @@
         <v>22</v>
       </c>
       <c r="P85" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="86" spans="1:16" ht="240" x14ac:dyDescent="0.25">
@@ -6058,7 +6058,7 @@
         <v>60</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C86">
         <v>4</v>
@@ -6094,10 +6094,10 @@
         <v>22</v>
       </c>
       <c r="O86" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="P86" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="87" spans="1:16" ht="285" x14ac:dyDescent="0.25">
@@ -6105,7 +6105,7 @@
         <v>61</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C87">
         <v>4</v>
@@ -6141,10 +6141,10 @@
         <v>22</v>
       </c>
       <c r="O87" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="P87" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="88" spans="1:16" ht="330" x14ac:dyDescent="0.25">
@@ -6152,7 +6152,7 @@
         <v>66</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C88">
         <v>4</v>
@@ -6188,7 +6188,7 @@
         <v>22</v>
       </c>
       <c r="P88" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="89" spans="1:16" ht="210" x14ac:dyDescent="0.25">
@@ -6196,7 +6196,7 @@
         <v>75</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C89">
         <v>4</v>
@@ -6232,7 +6232,7 @@
         <v>22</v>
       </c>
       <c r="P89" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="90" spans="1:16" ht="165" x14ac:dyDescent="0.25">
@@ -6240,7 +6240,7 @@
         <v>79</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C90">
         <v>4</v>
@@ -6276,7 +6276,7 @@
         <v>22</v>
       </c>
       <c r="P90" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="91" spans="1:16" ht="240" x14ac:dyDescent="0.25">
@@ -6284,7 +6284,7 @@
         <v>82</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C91">
         <v>4</v>
@@ -6320,7 +6320,7 @@
         <v>22</v>
       </c>
       <c r="P91" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="92" spans="1:16" ht="210" x14ac:dyDescent="0.25">
@@ -6328,7 +6328,7 @@
         <v>84</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C92">
         <v>6</v>
@@ -6364,7 +6364,7 @@
         <v>22</v>
       </c>
       <c r="P92" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="93" spans="1:16" ht="240" x14ac:dyDescent="0.25">
@@ -6372,7 +6372,7 @@
         <v>87</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C93">
         <v>6</v>
@@ -6408,7 +6408,7 @@
         <v>22</v>
       </c>
       <c r="P93" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="94" spans="1:16" ht="255" x14ac:dyDescent="0.25">
@@ -6416,7 +6416,7 @@
         <v>88</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C94">
         <v>6</v>
@@ -6452,7 +6452,7 @@
         <v>22</v>
       </c>
       <c r="P94" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="95" spans="1:16" ht="270" x14ac:dyDescent="0.25">
@@ -6460,7 +6460,7 @@
         <v>91</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C95">
         <v>4</v>
@@ -6496,10 +6496,10 @@
         <v>22</v>
       </c>
       <c r="O95" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="P95" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="96" spans="1:16" ht="315" x14ac:dyDescent="0.25">
@@ -6507,7 +6507,7 @@
         <v>94</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C96">
         <v>4</v>
@@ -6543,7 +6543,7 @@
         <v>22</v>
       </c>
       <c r="P96" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="97" spans="1:16" ht="270" x14ac:dyDescent="0.25">
@@ -6551,7 +6551,7 @@
         <v>96</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C97">
         <v>4</v>
@@ -6587,7 +6587,7 @@
         <v>22</v>
       </c>
       <c r="P97" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="98" spans="1:16" ht="330" x14ac:dyDescent="0.25">
@@ -6595,7 +6595,7 @@
         <v>101</v>
       </c>
       <c r="B98" s="3" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C98">
         <v>4</v>
@@ -6631,10 +6631,10 @@
         <v>22</v>
       </c>
       <c r="O98" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="P98" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="99" spans="1:16" ht="270" x14ac:dyDescent="0.25">
@@ -6642,7 +6642,7 @@
         <v>103</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C99" s="6">
         <v>6</v>
@@ -6678,7 +6678,7 @@
         <v>22</v>
       </c>
       <c r="P99" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="100" spans="1:16" ht="315" x14ac:dyDescent="0.25">
@@ -6686,7 +6686,7 @@
         <v>104</v>
       </c>
       <c r="B100" s="3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C100">
         <v>4</v>
@@ -6722,10 +6722,10 @@
         <v>22</v>
       </c>
       <c r="O100" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="P100" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="101" spans="1:16" x14ac:dyDescent="0.25">
@@ -6763,15 +6763,15 @@
         <v>22</v>
       </c>
       <c r="P101" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="102" spans="1:16" ht="135" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
+        <v>204</v>
+      </c>
+      <c r="B102" s="2" t="s">
         <v>205</v>
-      </c>
-      <c r="B102" s="2" t="s">
-        <v>206</v>
       </c>
       <c r="C102">
         <v>4</v>
@@ -6780,15 +6780,15 @@
         <v>11</v>
       </c>
       <c r="P102" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="103" spans="1:16" ht="390" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B103" s="2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C103">
         <v>4</v>
@@ -6797,18 +6797,18 @@
         <v>30</v>
       </c>
       <c r="O103" s="2" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="P103" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="104" spans="1:16" ht="330" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B104" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C104">
         <v>4</v>
@@ -6817,18 +6817,18 @@
         <v>22</v>
       </c>
       <c r="O104" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="P104" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="105" spans="1:16" ht="240" x14ac:dyDescent="0.25">
       <c r="A105" s="4" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B105" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C105">
         <v>2</v>
@@ -6837,18 +6837,18 @@
         <v>18</v>
       </c>
       <c r="O105" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="P105" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="106" spans="1:16" ht="90" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
+        <v>215</v>
+      </c>
+      <c r="B106" s="2" t="s">
         <v>216</v>
-      </c>
-      <c r="B106" s="2" t="s">
-        <v>217</v>
       </c>
       <c r="C106">
         <v>4</v>
@@ -6857,10 +6857,10 @@
         <v>13</v>
       </c>
       <c r="O106" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="P106" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
   </sheetData>

</xml_diff>